<commit_message>
ajustando pipe com NLP
</commit_message>
<xml_diff>
--- a/config/modelos/frames_nf_v11.xlsx
+++ b/config/modelos/frames_nf_v11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\dani-boy\extractNF\config\modelos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E44C38-3841-433E-B715-FE7AAE7ED3EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{671C98AC-BAAE-4553-90AD-FDADC22FF069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2501" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2507" uniqueCount="195">
   <si>
     <t>id</t>
   </si>
@@ -1081,10 +1081,10 @@
   <dimension ref="A1:AH232"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1107,7 +1107,7 @@
     <col min="17" max="17" width="41.7265625" customWidth="1"/>
     <col min="18" max="18" width="27.453125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="21.36328125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="27.453125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="24.08984375" customWidth="1"/>
     <col min="21" max="24" width="5.7265625" customWidth="1"/>
     <col min="25" max="25" width="7.08984375" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="6" bestFit="1" customWidth="1"/>
@@ -1237,7 +1237,7 @@
         <v>32</v>
       </c>
       <c r="E2" s="16">
-        <v>2.4</v>
+        <v>2.5</v>
       </c>
       <c r="F2" s="11">
         <v>1</v>
@@ -1827,16 +1827,16 @@
       <c r="S9" s="14"/>
       <c r="T9" s="14"/>
       <c r="U9" s="14">
-        <v>3285</v>
+        <v>3210</v>
       </c>
       <c r="V9" s="14">
-        <v>176</v>
+        <v>229</v>
       </c>
       <c r="W9" s="14">
-        <v>3874</v>
+        <v>3806</v>
       </c>
       <c r="X9" s="14">
-        <v>780</v>
+        <v>806</v>
       </c>
       <c r="Y9" s="14">
         <v>434</v>
@@ -4763,8 +4763,12 @@
       <c r="G46" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="H46" s="14"/>
-      <c r="I46" s="15"/>
+      <c r="H46" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="I46" s="15" t="s">
+        <v>190</v>
+      </c>
       <c r="J46" s="14" t="s">
         <v>43</v>
       </c>
@@ -4839,8 +4843,12 @@
       <c r="G47" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H47" s="7"/>
-      <c r="I47" s="8"/>
+      <c r="H47" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="I47" s="8" t="s">
+        <v>190</v>
+      </c>
       <c r="J47" s="7" t="s">
         <v>45</v>
       </c>
@@ -4929,8 +4937,12 @@
       <c r="G48" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H48" s="7"/>
-      <c r="I48" s="8"/>
+      <c r="H48" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="I48" s="8" t="s">
+        <v>190</v>
+      </c>
       <c r="J48" s="7" t="s">
         <v>45</v>
       </c>

</xml_diff>